<commit_message>
Atualização funções (atualização anexo F, correção form.html)
</commit_message>
<xml_diff>
--- a/gerados/anexo_f_preenchido.xlsx
+++ b/gerados/anexo_f_preenchido.xlsx
@@ -223,9 +223,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -235,55 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -292,6 +241,57 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="justify" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -701,8 +701,8 @@
   </sheetPr>
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A120" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G127" sqref="G127"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -710,27 +710,27 @@
     <col width="35.140625" customWidth="1" style="2" min="1" max="1"/>
     <col width="21.42578125" customWidth="1" style="2" min="2" max="3"/>
     <col width="16.7109375" customWidth="1" style="2" min="4" max="5"/>
-    <col width="14.5703125" customWidth="1" style="24" min="6" max="6"/>
+    <col width="14.5703125" customWidth="1" style="37" min="6" max="6"/>
     <col width="14.5703125" customWidth="1" style="2" min="7" max="8"/>
     <col width="8.85546875" customWidth="1" style="2" min="9" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="201.75" customHeight="1">
-      <c r="A1" s="38" t="inlineStr">
+      <c r="A1" s="21" t="inlineStr">
         <is>
           <t>ANEXO F – Dados para Registro de Micro e Minigeradores Distribuídos Participantes do Sistema de Compensação de Energia Elétrica
 Na ocasião da Solicitação de Acesso, as informações pedidas para este Anexo F são mandatórias e serão remetidas pela CPFL à ANEEL, conforme por esta próprio determinado, após a liberação da conexão. O consumidor deverá estar ciente de que a citada liberação também depende do correto preenchimento do que aqui se solicita. Este refere-se a cada unidade consumidora que tiver aprovada central de micro ou minigeração distribuída aderente ao sistema de compensação de energia elétrica e deverá ser preenchida pelo consumidor (deixar em branco o que não se aplicar). 
 Na ocasião da Consulta de Acesso é incentivado que o consumidor envie este anexo preenchido, em especial os itens marcados com asterisco. Somente com as informações destes itens será possível avaliar a viabilidade e estimar as obras em virtude da conexão de minigeradores. Sem eles, a Informação de Acesso da CPFL conterá apenas os dados elétricos da região em que se pretende conexão.</t>
         </is>
       </c>
-      <c r="F1" s="24" t="n"/>
+      <c r="F1" s="37" t="n"/>
     </row>
     <row r="2">
       <c r="C2" s="1" t="n"/>
-      <c r="F2" s="24" t="n"/>
+      <c r="F2" s="37" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="30" t="inlineStr">
+      <c r="A3" s="22" t="inlineStr">
         <is>
           <t>1) Dados da Unidade Consumidora (UC):</t>
         </is>
@@ -739,7 +739,7 @@
       <c r="C3" s="39" t="n"/>
       <c r="D3" s="39" t="n"/>
       <c r="E3" s="40" t="n"/>
-      <c r="F3" s="24" t="n"/>
+      <c r="F3" s="37" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="8" t="inlineStr">
@@ -747,7 +747,7 @@
           <t>1.1) Nome do titular: *</t>
         </is>
       </c>
-      <c r="B4" s="37" t="inlineStr">
+      <c r="B4" s="20" t="inlineStr">
         <is>
           <t>Joao marques Rantary</t>
         </is>
@@ -755,7 +755,7 @@
       <c r="C4" s="41" t="n"/>
       <c r="D4" s="41" t="n"/>
       <c r="E4" s="42" t="n"/>
-      <c r="F4" s="24" t="n"/>
+      <c r="F4" s="37" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="8" t="inlineStr">
@@ -763,7 +763,7 @@
           <t>1.2) CNPJ ou CPF (titular): *</t>
         </is>
       </c>
-      <c r="B5" s="37" t="inlineStr">
+      <c r="B5" s="20" t="inlineStr">
         <is>
           <t>446.790.168-09</t>
         </is>
@@ -771,7 +771,7 @@
       <c r="C5" s="41" t="n"/>
       <c r="D5" s="41" t="n"/>
       <c r="E5" s="42" t="n"/>
-      <c r="F5" s="24" t="n"/>
+      <c r="F5" s="37" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="8" t="inlineStr">
@@ -779,7 +779,7 @@
           <t>1.3) Número da UC (se existente) *</t>
         </is>
       </c>
-      <c r="B6" s="37" t="inlineStr">
+      <c r="B6" s="20" t="inlineStr">
         <is>
           <t>#UC</t>
         </is>
@@ -787,7 +787,7 @@
       <c r="C6" s="41" t="n"/>
       <c r="D6" s="41" t="n"/>
       <c r="E6" s="42" t="n"/>
-      <c r="F6" s="24" t="n"/>
+      <c r="F6" s="37" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="8" t="inlineStr">
@@ -795,7 +795,7 @@
           <t>1.4) Endereço do titular</t>
         </is>
       </c>
-      <c r="B7" s="37" t="inlineStr">
+      <c r="B7" s="20" t="inlineStr">
         <is>
           <t>Avenida São José do Rio Preto, 3730</t>
         </is>
@@ -803,7 +803,7 @@
       <c r="C7" s="41" t="n"/>
       <c r="D7" s="41" t="n"/>
       <c r="E7" s="42" t="n"/>
-      <c r="F7" s="24" t="n"/>
+      <c r="F7" s="37" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="8" t="inlineStr">
@@ -811,7 +811,7 @@
           <t>1.5) CEP do titular</t>
         </is>
       </c>
-      <c r="B8" s="37" t="inlineStr">
+      <c r="B8" s="20" t="inlineStr">
         <is>
           <t>#CEP</t>
         </is>
@@ -819,7 +819,7 @@
       <c r="C8" s="41" t="n"/>
       <c r="D8" s="41" t="n"/>
       <c r="E8" s="42" t="n"/>
-      <c r="F8" s="24" t="n"/>
+      <c r="F8" s="37" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="8" t="inlineStr">
@@ -827,7 +827,7 @@
           <t>1.6) Município do titular</t>
         </is>
       </c>
-      <c r="B9" s="37" t="inlineStr">
+      <c r="B9" s="20" t="inlineStr">
         <is>
           <t>São José do Rio Preto</t>
         </is>
@@ -835,7 +835,7 @@
       <c r="C9" s="41" t="n"/>
       <c r="D9" s="41" t="n"/>
       <c r="E9" s="42" t="n"/>
-      <c r="F9" s="24" t="n"/>
+      <c r="F9" s="37" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="8" t="inlineStr">
@@ -843,7 +843,7 @@
           <t>1.7) Latitude (SIRGAS 2000)</t>
         </is>
       </c>
-      <c r="B10" s="37" t="inlineStr">
+      <c r="B10" s="20" t="inlineStr">
         <is>
           <t>#LAT</t>
         </is>
@@ -851,7 +851,7 @@
       <c r="C10" s="41" t="n"/>
       <c r="D10" s="41" t="n"/>
       <c r="E10" s="42" t="n"/>
-      <c r="F10" s="24" t="n"/>
+      <c r="F10" s="37" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="8" t="inlineStr">
@@ -859,7 +859,7 @@
           <t>1.8) Longitude (SIRGAS 2000)</t>
         </is>
       </c>
-      <c r="B11" s="37" t="inlineStr">
+      <c r="B11" s="20" t="inlineStr">
         <is>
           <t>#LONG</t>
         </is>
@@ -867,7 +867,7 @@
       <c r="C11" s="41" t="n"/>
       <c r="D11" s="41" t="n"/>
       <c r="E11" s="42" t="n"/>
-      <c r="F11" s="24" t="n"/>
+      <c r="F11" s="37" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="8" t="inlineStr">
@@ -875,7 +875,7 @@
           <t>1.7) Telefone do titular:</t>
         </is>
       </c>
-      <c r="B12" s="37" t="inlineStr">
+      <c r="B12" s="20" t="inlineStr">
         <is>
           <t>#TEL</t>
         </is>
@@ -883,7 +883,7 @@
       <c r="C12" s="41" t="n"/>
       <c r="D12" s="41" t="n"/>
       <c r="E12" s="42" t="n"/>
-      <c r="F12" s="24" t="n"/>
+      <c r="F12" s="37" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="8" t="inlineStr">
@@ -891,7 +891,7 @@
           <t>1.8) E-mail do titular:</t>
         </is>
       </c>
-      <c r="B13" s="37" t="inlineStr">
+      <c r="B13" s="20" t="inlineStr">
         <is>
           <t>#CEL</t>
         </is>
@@ -899,7 +899,7 @@
       <c r="C13" s="41" t="n"/>
       <c r="D13" s="41" t="n"/>
       <c r="E13" s="42" t="n"/>
-      <c r="F13" s="24" t="n"/>
+      <c r="F13" s="37" t="n"/>
     </row>
     <row r="14" ht="30" customHeight="1">
       <c r="A14" s="8" t="inlineStr">
@@ -907,11 +907,11 @@
           <t>1.9) Usina foi objeto de Outorga ou Registro?</t>
         </is>
       </c>
-      <c r="B14" s="37" t="n"/>
+      <c r="B14" s="20" t="n"/>
       <c r="C14" s="41" t="n"/>
       <c r="D14" s="41" t="n"/>
       <c r="E14" s="42" t="n"/>
-      <c r="F14" s="20" t="inlineStr">
+      <c r="F14" s="34" t="inlineStr">
         <is>
           <t>* se sim, preencher os campos abaixo</t>
         </is>
@@ -923,11 +923,11 @@
           <t>1.10) CEG</t>
         </is>
       </c>
-      <c r="B15" s="37" t="n"/>
+      <c r="B15" s="20" t="n"/>
       <c r="C15" s="41" t="n"/>
       <c r="D15" s="41" t="n"/>
       <c r="E15" s="42" t="n"/>
-      <c r="F15" s="24" t="n"/>
+      <c r="F15" s="37" t="n"/>
     </row>
     <row r="16" ht="30" customHeight="1">
       <c r="A16" s="8" t="inlineStr">
@@ -935,11 +935,11 @@
           <t>1.11) Número do Ato de Outorga ou Registro</t>
         </is>
       </c>
-      <c r="B16" s="37" t="n"/>
+      <c r="B16" s="20" t="n"/>
       <c r="C16" s="41" t="n"/>
       <c r="D16" s="41" t="n"/>
       <c r="E16" s="42" t="n"/>
-      <c r="F16" s="24" t="n"/>
+      <c r="F16" s="37" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="8" t="inlineStr">
@@ -947,11 +947,11 @@
           <t>1.12) Nome da Usina:</t>
         </is>
       </c>
-      <c r="B17" s="37" t="n"/>
+      <c r="B17" s="20" t="n"/>
       <c r="C17" s="41" t="n"/>
       <c r="D17" s="41" t="n"/>
       <c r="E17" s="42" t="n"/>
-      <c r="F17" s="24" t="n"/>
+      <c r="F17" s="37" t="n"/>
     </row>
     <row r="18" ht="30" customHeight="1">
       <c r="A18" s="8" t="inlineStr">
@@ -959,11 +959,11 @@
           <t>1.13) Ano do Ato de Outorga ou Registro</t>
         </is>
       </c>
-      <c r="B18" s="37" t="n"/>
+      <c r="B18" s="20" t="n"/>
       <c r="C18" s="41" t="n"/>
       <c r="D18" s="41" t="n"/>
       <c r="E18" s="42" t="n"/>
-      <c r="F18" s="24" t="n"/>
+      <c r="F18" s="37" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="15" t="n"/>
@@ -971,7 +971,7 @@
       <c r="C19" s="39" t="n"/>
       <c r="D19" s="39" t="n"/>
       <c r="E19" s="40" t="n"/>
-      <c r="F19" s="24" t="n"/>
+      <c r="F19" s="37" t="n"/>
     </row>
     <row r="20" ht="30" customHeight="1">
       <c r="A20" s="3" t="inlineStr">
@@ -980,19 +980,19 @@
 Consumidora (se Microgeração) </t>
         </is>
       </c>
-      <c r="B20" s="34" t="inlineStr">
+      <c r="B20" s="24" t="inlineStr">
         <is>
           <t>Existente</t>
         </is>
       </c>
       <c r="C20" s="40" t="n"/>
-      <c r="D20" s="34" t="inlineStr">
+      <c r="D20" s="24" t="inlineStr">
         <is>
           <t>Novo</t>
         </is>
       </c>
       <c r="E20" s="40" t="n"/>
-      <c r="F20" s="24" t="n"/>
+      <c r="F20" s="37" t="n"/>
     </row>
     <row r="21" ht="30" customHeight="1">
       <c r="A21" s="8" t="inlineStr">
@@ -1000,11 +1000,15 @@
           <t>2.1) Padrão de Entrada (categoria - GED 13/RIC BT):</t>
         </is>
       </c>
-      <c r="B21" s="22" t="n"/>
+      <c r="B21" s="23" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
       <c r="C21" s="40" t="n"/>
-      <c r="D21" s="22" t="n"/>
+      <c r="D21" s="23" t="n"/>
       <c r="E21" s="40" t="n"/>
-      <c r="F21" s="24" t="n"/>
+      <c r="F21" s="37" t="n"/>
     </row>
     <row r="22" ht="30" customHeight="1">
       <c r="A22" s="8" t="inlineStr">
@@ -1012,11 +1016,15 @@
           <t>2.2) Tipo de Atendimento (aéreo/subterrâneo):</t>
         </is>
       </c>
-      <c r="B22" s="22" t="n"/>
+      <c r="B22" s="23" t="inlineStr">
+        <is>
+          <t>Aérea</t>
+        </is>
+      </c>
       <c r="C22" s="40" t="n"/>
-      <c r="D22" s="22" t="n"/>
+      <c r="D22" s="23" t="n"/>
       <c r="E22" s="40" t="n"/>
-      <c r="F22" s="24" t="n"/>
+      <c r="F22" s="37" t="n"/>
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" s="8" t="inlineStr">
@@ -1024,9 +1032,13 @@
           <t>2.3) Número de Fases da Instalação (Monofásico/Bifásico/Trifásico):</t>
         </is>
       </c>
-      <c r="B23" s="22" t="n"/>
+      <c r="B23" s="23" t="inlineStr">
+        <is>
+          <t>Bifásico</t>
+        </is>
+      </c>
       <c r="C23" s="40" t="n"/>
-      <c r="D23" s="22" t="n"/>
+      <c r="D23" s="23" t="n"/>
       <c r="E23" s="40" t="n"/>
       <c r="F23" s="7" t="n"/>
       <c r="G23" s="6" t="n"/>
@@ -1040,11 +1052,15 @@
           <t>2.4) Cabos (seção transversal):</t>
         </is>
       </c>
-      <c r="B24" s="22" t="n"/>
+      <c r="B24" s="23" t="inlineStr">
+        <is>
+          <t>16 mm²</t>
+        </is>
+      </c>
       <c r="C24" s="40" t="n"/>
-      <c r="D24" s="22" t="n"/>
+      <c r="D24" s="23" t="n"/>
       <c r="E24" s="40" t="n"/>
-      <c r="F24" s="24" t="n"/>
+      <c r="F24" s="37" t="n"/>
     </row>
     <row r="25" ht="45" customHeight="1">
       <c r="A25" s="8" t="inlineStr">
@@ -1052,11 +1068,15 @@
           <t>2.5) Caixa de Medição ou Tipo de Poste Padrão (Caixa tipo, segundo GED 14945):</t>
         </is>
       </c>
-      <c r="B25" s="22" t="n"/>
+      <c r="B25" s="23" t="inlineStr">
+        <is>
+          <t>II</t>
+        </is>
+      </c>
       <c r="C25" s="40" t="n"/>
-      <c r="D25" s="22" t="n"/>
+      <c r="D25" s="23" t="n"/>
       <c r="E25" s="40" t="n"/>
-      <c r="F25" s="24" t="n"/>
+      <c r="F25" s="37" t="n"/>
     </row>
     <row r="26" ht="30" customHeight="1">
       <c r="A26" s="8" t="inlineStr">
@@ -1064,11 +1084,15 @@
           <t>2.6) Demanda Disponibilizada (se MT) ou Carga Instalada (se BT):</t>
         </is>
       </c>
-      <c r="B26" s="22" t="n"/>
+      <c r="B26" s="23" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="C26" s="40" t="n"/>
-      <c r="D26" s="22" t="n"/>
+      <c r="D26" s="23" t="n"/>
       <c r="E26" s="40" t="n"/>
-      <c r="F26" s="24" t="n"/>
+      <c r="F26" s="37" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="8" t="inlineStr">
@@ -1076,11 +1100,15 @@
           <t>2.7) Disjuntor (A):</t>
         </is>
       </c>
-      <c r="B27" s="22" t="n"/>
+      <c r="B27" s="23" t="inlineStr">
+        <is>
+          <t>63A</t>
+        </is>
+      </c>
       <c r="C27" s="40" t="n"/>
-      <c r="D27" s="22" t="n"/>
+      <c r="D27" s="23" t="n"/>
       <c r="E27" s="40" t="n"/>
-      <c r="F27" s="24" t="n"/>
+      <c r="F27" s="37" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="15" t="n"/>
@@ -1088,7 +1116,7 @@
       <c r="C28" s="39" t="n"/>
       <c r="D28" s="39" t="n"/>
       <c r="E28" s="40" t="n"/>
-      <c r="F28" s="24" t="n"/>
+      <c r="F28" s="37" t="n"/>
     </row>
     <row r="29" ht="30" customHeight="1">
       <c r="A29" s="3" t="inlineStr">
@@ -1096,23 +1124,23 @@
           <t>2b) Dados Técnicos da Unidade Consumidora (se Minigeração)</t>
         </is>
       </c>
-      <c r="B29" s="34" t="inlineStr">
+      <c r="B29" s="24" t="inlineStr">
         <is>
           <t>Situação Atual</t>
         </is>
       </c>
-      <c r="C29" s="34" t="inlineStr">
+      <c r="C29" s="24" t="inlineStr">
         <is>
           <t>Acréscimo</t>
         </is>
       </c>
-      <c r="D29" s="34" t="inlineStr">
+      <c r="D29" s="24" t="inlineStr">
         <is>
           <t>Total Previsto</t>
         </is>
       </c>
       <c r="E29" s="40" t="n"/>
-      <c r="F29" s="24" t="n"/>
+      <c r="F29" s="37" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="12" t="inlineStr">
@@ -1122,9 +1150,9 @@
       </c>
       <c r="B30" s="13" t="n"/>
       <c r="C30" s="13" t="n"/>
-      <c r="D30" s="36" t="n"/>
+      <c r="D30" s="28" t="n"/>
       <c r="E30" s="40" t="n"/>
-      <c r="F30" s="24" t="n"/>
+      <c r="F30" s="37" t="n"/>
     </row>
     <row r="31" ht="30" customHeight="1">
       <c r="A31" s="12" t="inlineStr">
@@ -1134,9 +1162,9 @@
       </c>
       <c r="B31" s="13" t="n"/>
       <c r="C31" s="13" t="n"/>
-      <c r="D31" s="36" t="n"/>
+      <c r="D31" s="28" t="n"/>
       <c r="E31" s="40" t="n"/>
-      <c r="F31" s="24" t="n"/>
+      <c r="F31" s="37" t="n"/>
     </row>
     <row r="32" ht="30" customHeight="1">
       <c r="A32" s="12" t="inlineStr">
@@ -1146,9 +1174,9 @@
       </c>
       <c r="B32" s="13" t="n"/>
       <c r="C32" s="13" t="n"/>
-      <c r="D32" s="36" t="n"/>
+      <c r="D32" s="28" t="n"/>
       <c r="E32" s="40" t="n"/>
-      <c r="F32" s="23" t="n"/>
+      <c r="F32" s="36" t="n"/>
     </row>
     <row r="33" ht="30" customHeight="1">
       <c r="A33" s="12" t="inlineStr">
@@ -1158,9 +1186,9 @@
       </c>
       <c r="B33" s="13" t="n"/>
       <c r="C33" s="13" t="n"/>
-      <c r="D33" s="36" t="n"/>
+      <c r="D33" s="28" t="n"/>
       <c r="E33" s="40" t="n"/>
-      <c r="F33" s="20" t="inlineStr">
+      <c r="F33" s="34" t="inlineStr">
         <is>
           <t>* O fator limitante da potência instalada de geração é o menor valor entre módulo e inversosr do projeto</t>
         </is>
@@ -1174,9 +1202,9 @@
       </c>
       <c r="B34" s="13" t="n"/>
       <c r="C34" s="13" t="n"/>
-      <c r="D34" s="36" t="n"/>
+      <c r="D34" s="28" t="n"/>
       <c r="E34" s="40" t="n"/>
-      <c r="F34" s="24" t="n"/>
+      <c r="F34" s="37" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="12" t="inlineStr">
@@ -1184,11 +1212,11 @@
           <t>2.6) Nome do responsável técnico: *</t>
         </is>
       </c>
-      <c r="B35" s="36" t="n"/>
+      <c r="B35" s="28" t="n"/>
       <c r="C35" s="39" t="n"/>
       <c r="D35" s="39" t="n"/>
       <c r="E35" s="40" t="n"/>
-      <c r="F35" s="24" t="n"/>
+      <c r="F35" s="37" t="n"/>
     </row>
     <row r="36" ht="30" customHeight="1">
       <c r="A36" s="12" t="inlineStr">
@@ -1196,11 +1224,11 @@
           <t>2.7) Número do registro (CREA) do responsável técnico: *</t>
         </is>
       </c>
-      <c r="B36" s="36" t="n"/>
+      <c r="B36" s="28" t="n"/>
       <c r="C36" s="39" t="n"/>
       <c r="D36" s="39" t="n"/>
       <c r="E36" s="40" t="n"/>
-      <c r="F36" s="24" t="n"/>
+      <c r="F36" s="37" t="n"/>
     </row>
     <row r="37" ht="30" customHeight="1">
       <c r="A37" s="12" t="inlineStr">
@@ -1208,11 +1236,11 @@
           <t>2.8) Número do telefone do responsável técnico:</t>
         </is>
       </c>
-      <c r="B37" s="36" t="n"/>
+      <c r="B37" s="28" t="n"/>
       <c r="C37" s="39" t="n"/>
       <c r="D37" s="39" t="n"/>
       <c r="E37" s="40" t="n"/>
-      <c r="F37" s="24" t="n"/>
+      <c r="F37" s="37" t="n"/>
     </row>
     <row r="38" ht="30" customHeight="1">
       <c r="A38" s="12" t="inlineStr">
@@ -1220,11 +1248,11 @@
           <t>2.9) Data pretendida para entrada em operação (dd/mm/aaaa):</t>
         </is>
       </c>
-      <c r="B38" s="36" t="n"/>
+      <c r="B38" s="28" t="n"/>
       <c r="C38" s="39" t="n"/>
       <c r="D38" s="39" t="n"/>
       <c r="E38" s="40" t="n"/>
-      <c r="F38" s="24" t="n"/>
+      <c r="F38" s="37" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="15" t="n"/>
@@ -1232,7 +1260,7 @@
       <c r="C39" s="39" t="n"/>
       <c r="D39" s="39" t="n"/>
       <c r="E39" s="40" t="n"/>
-      <c r="F39" s="24" t="n"/>
+      <c r="F39" s="37" t="n"/>
     </row>
     <row r="40" ht="30" customHeight="1">
       <c r="A40" s="3" t="inlineStr">
@@ -1260,43 +1288,43 @@
           <t>T4</t>
         </is>
       </c>
-      <c r="F40" s="24" t="n"/>
+      <c r="F40" s="37" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="25" t="inlineStr">
+      <c r="A41" s="38" t="inlineStr">
         <is>
           <t>2.1) Potência Nominal (kVA): *</t>
         </is>
       </c>
-      <c r="B41" s="25" t="n"/>
-      <c r="C41" s="25" t="n"/>
-      <c r="D41" s="25" t="n"/>
-      <c r="E41" s="25" t="n"/>
-      <c r="F41" s="24" t="n"/>
+      <c r="B41" s="38" t="n"/>
+      <c r="C41" s="38" t="n"/>
+      <c r="D41" s="38" t="n"/>
+      <c r="E41" s="38" t="n"/>
+      <c r="F41" s="37" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="25" t="inlineStr">
+      <c r="A42" s="38" t="inlineStr">
         <is>
           <t>2.2) Tensão Primária (kV): *</t>
         </is>
       </c>
-      <c r="B42" s="25" t="n"/>
-      <c r="C42" s="25" t="n"/>
-      <c r="D42" s="25" t="n"/>
-      <c r="E42" s="25" t="n"/>
-      <c r="F42" s="24" t="n"/>
+      <c r="B42" s="38" t="n"/>
+      <c r="C42" s="38" t="n"/>
+      <c r="D42" s="38" t="n"/>
+      <c r="E42" s="38" t="n"/>
+      <c r="F42" s="37" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="25" t="inlineStr">
+      <c r="A43" s="38" t="inlineStr">
         <is>
           <t>2.3) Tensão Secundária (V): *</t>
         </is>
       </c>
-      <c r="B43" s="25" t="n"/>
-      <c r="C43" s="25" t="n"/>
-      <c r="D43" s="25" t="n"/>
-      <c r="E43" s="25" t="n"/>
-      <c r="F43" s="24" t="n"/>
+      <c r="B43" s="38" t="n"/>
+      <c r="C43" s="38" t="n"/>
+      <c r="D43" s="38" t="n"/>
+      <c r="E43" s="38" t="n"/>
+      <c r="F43" s="37" t="n"/>
     </row>
     <row r="44" ht="30" customHeight="1">
       <c r="A44" s="8" t="inlineStr">
@@ -1304,11 +1332,11 @@
           <t>2.4) Impedância de curto-circuito (Z%): *</t>
         </is>
       </c>
-      <c r="B44" s="25" t="n"/>
-      <c r="C44" s="25" t="n"/>
-      <c r="D44" s="25" t="n"/>
-      <c r="E44" s="25" t="n"/>
-      <c r="F44" s="24" t="n"/>
+      <c r="B44" s="38" t="n"/>
+      <c r="C44" s="38" t="n"/>
+      <c r="D44" s="38" t="n"/>
+      <c r="E44" s="38" t="n"/>
+      <c r="F44" s="37" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="8" t="inlineStr">
@@ -1316,11 +1344,11 @@
           <t>2.5) Configuração de ligação: *</t>
         </is>
       </c>
-      <c r="B45" s="25" t="n"/>
-      <c r="C45" s="25" t="n"/>
-      <c r="D45" s="25" t="n"/>
-      <c r="E45" s="25" t="n"/>
-      <c r="F45" s="24" t="n"/>
+      <c r="B45" s="38" t="n"/>
+      <c r="C45" s="38" t="n"/>
+      <c r="D45" s="38" t="n"/>
+      <c r="E45" s="38" t="n"/>
+      <c r="F45" s="37" t="n"/>
     </row>
     <row r="46" ht="30" customHeight="1">
       <c r="A46" s="8" t="inlineStr">
@@ -1328,11 +1356,11 @@
           <t>2.6) Tensão de geração/Saída do inversor (Vca): *</t>
         </is>
       </c>
-      <c r="B46" s="25" t="n"/>
-      <c r="C46" s="25" t="n"/>
-      <c r="D46" s="25" t="n"/>
-      <c r="E46" s="25" t="n"/>
-      <c r="F46" s="24" t="n"/>
+      <c r="B46" s="38" t="n"/>
+      <c r="C46" s="38" t="n"/>
+      <c r="D46" s="38" t="n"/>
+      <c r="E46" s="38" t="n"/>
+      <c r="F46" s="37" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="9" t="n"/>
@@ -1340,7 +1368,7 @@
       <c r="C47" s="10" t="n"/>
       <c r="D47" s="10" t="n"/>
       <c r="E47" s="11" t="n"/>
-      <c r="F47" s="24" t="n"/>
+      <c r="F47" s="37" t="n"/>
     </row>
     <row r="48" ht="30" customHeight="1">
       <c r="A48" s="3" t="inlineStr">
@@ -1348,147 +1376,147 @@
           <t>2d) Dados do Sistema de Armazenamento de Energia (SAE)</t>
         </is>
       </c>
-      <c r="B48" s="34" t="inlineStr">
+      <c r="B48" s="24" t="inlineStr">
         <is>
           <t>Situação Atual</t>
         </is>
       </c>
-      <c r="C48" s="34" t="inlineStr">
+      <c r="C48" s="24" t="inlineStr">
         <is>
           <t>Acréscimo</t>
         </is>
       </c>
-      <c r="D48" s="34" t="inlineStr">
+      <c r="D48" s="24" t="inlineStr">
         <is>
           <t>Total Previsto</t>
         </is>
       </c>
       <c r="E48" s="40" t="n"/>
-      <c r="F48" s="24" t="n"/>
+      <c r="F48" s="37" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="25" t="inlineStr">
+      <c r="A49" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">2.1) Tipo do SAE: </t>
         </is>
       </c>
       <c r="B49" s="15" t="n"/>
       <c r="C49" s="15" t="n"/>
-      <c r="D49" s="22" t="inlineStr">
+      <c r="D49" s="23" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E49" s="40" t="n"/>
-      <c r="F49" s="24" t="n"/>
+      <c r="F49" s="37" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="25" t="inlineStr">
+      <c r="A50" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">2.2) Potência Nominal (kW): </t>
         </is>
       </c>
-      <c r="B50" s="25" t="n"/>
-      <c r="C50" s="25" t="n"/>
-      <c r="D50" s="22" t="n"/>
+      <c r="B50" s="38" t="n"/>
+      <c r="C50" s="38" t="n"/>
+      <c r="D50" s="23" t="n"/>
       <c r="E50" s="40" t="n"/>
-      <c r="F50" s="24" t="n"/>
+      <c r="F50" s="37" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" s="25" t="inlineStr">
+      <c r="A51" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">2.3) Energia (kWh): </t>
         </is>
       </c>
-      <c r="B51" s="25" t="n"/>
-      <c r="C51" s="25" t="n"/>
-      <c r="D51" s="22" t="n"/>
+      <c r="B51" s="38" t="n"/>
+      <c r="C51" s="38" t="n"/>
+      <c r="D51" s="23" t="n"/>
       <c r="E51" s="40" t="n"/>
-      <c r="F51" s="24" t="n"/>
+      <c r="F51" s="37" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="25" t="inlineStr">
+      <c r="A52" s="38" t="inlineStr">
         <is>
           <t>2.4) Listar fabricantes:</t>
         </is>
       </c>
-      <c r="B52" s="25" t="n"/>
-      <c r="C52" s="25" t="n"/>
-      <c r="D52" s="22" t="inlineStr">
+      <c r="B52" s="38" t="n"/>
+      <c r="C52" s="38" t="n"/>
+      <c r="D52" s="23" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E52" s="40" t="n"/>
-      <c r="F52" s="24" t="n"/>
+      <c r="F52" s="37" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="25" t="inlineStr">
+      <c r="A53" s="38" t="inlineStr">
         <is>
           <t>2.5) Listar modelos:</t>
         </is>
       </c>
-      <c r="B53" s="25" t="n"/>
-      <c r="C53" s="25" t="n"/>
-      <c r="D53" s="22" t="inlineStr">
+      <c r="B53" s="38" t="n"/>
+      <c r="C53" s="38" t="n"/>
+      <c r="D53" s="23" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E53" s="40" t="n"/>
-      <c r="F53" s="24" t="n"/>
+      <c r="F53" s="37" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="25" t="inlineStr">
+      <c r="A54" s="38" t="inlineStr">
         <is>
           <t>2.6) Quantidade total de inversores: *</t>
         </is>
       </c>
-      <c r="B54" s="25" t="n"/>
-      <c r="C54" s="25" t="n"/>
-      <c r="D54" s="22" t="n"/>
+      <c r="B54" s="38" t="n"/>
+      <c r="C54" s="38" t="n"/>
+      <c r="D54" s="23" t="n"/>
       <c r="E54" s="40" t="n"/>
-      <c r="F54" s="21" t="inlineStr">
+      <c r="F54" s="35" t="inlineStr">
         <is>
           <t>*Caso aplicável</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="25" t="inlineStr">
+      <c r="A55" s="38" t="inlineStr">
         <is>
           <t>2.7) Listar fabricantes dos inversores: *</t>
         </is>
       </c>
-      <c r="B55" s="25" t="n"/>
-      <c r="C55" s="25" t="n"/>
-      <c r="D55" s="22" t="inlineStr">
+      <c r="B55" s="38" t="n"/>
+      <c r="C55" s="38" t="n"/>
+      <c r="D55" s="23" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E55" s="40" t="n"/>
-      <c r="F55" s="21" t="inlineStr">
+      <c r="F55" s="35" t="inlineStr">
         <is>
           <t>*Caso aplicável</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="25" t="inlineStr">
+      <c r="A56" s="38" t="inlineStr">
         <is>
           <t>2.8) Listar modelos dos inversores: *</t>
         </is>
       </c>
-      <c r="B56" s="25" t="n"/>
-      <c r="C56" s="25" t="n"/>
-      <c r="D56" s="22" t="inlineStr">
+      <c r="B56" s="38" t="n"/>
+      <c r="C56" s="38" t="n"/>
+      <c r="D56" s="23" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
       <c r="E56" s="40" t="n"/>
-      <c r="F56" s="21" t="inlineStr">
+      <c r="F56" s="35" t="inlineStr">
         <is>
           <t>*Caso aplicável</t>
         </is>
@@ -1500,11 +1528,11 @@
           <t>2.9) Potência Nominal dos inversores (soma das potências nominais dos inversores, kW): *</t>
         </is>
       </c>
-      <c r="B57" s="25" t="n"/>
-      <c r="C57" s="25" t="n"/>
-      <c r="D57" s="22" t="n"/>
+      <c r="B57" s="38" t="n"/>
+      <c r="C57" s="38" t="n"/>
+      <c r="D57" s="23" t="n"/>
       <c r="E57" s="40" t="n"/>
-      <c r="F57" s="21" t="inlineStr">
+      <c r="F57" s="35" t="inlineStr">
         <is>
           <t>*Caso aplicável</t>
         </is>
@@ -1516,7 +1544,7 @@
       <c r="C58" s="10" t="n"/>
       <c r="D58" s="10" t="n"/>
       <c r="E58" s="11" t="n"/>
-      <c r="F58" s="24" t="n"/>
+      <c r="F58" s="37" t="n"/>
     </row>
     <row r="59" ht="30" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
@@ -1534,61 +1562,61 @@
           <t>Acréscimo</t>
         </is>
       </c>
-      <c r="D59" s="34" t="inlineStr">
+      <c r="D59" s="24" t="inlineStr">
         <is>
           <t>Total Previsto</t>
         </is>
       </c>
       <c r="E59" s="40" t="n"/>
-      <c r="F59" s="24" t="n"/>
+      <c r="F59" s="37" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" s="25" t="inlineStr">
+      <c r="A60" s="38" t="inlineStr">
         <is>
           <t>3.1) Quantidade total de módulos:</t>
         </is>
       </c>
-      <c r="B60" s="25" t="inlineStr">
+      <c r="B60" s="38" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="C60" s="25" t="n"/>
-      <c r="D60" s="22" t="n"/>
+      <c r="C60" s="38" t="n"/>
+      <c r="D60" s="23" t="n"/>
       <c r="E60" s="40" t="n"/>
-      <c r="F60" s="24" t="n"/>
+      <c r="F60" s="37" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" s="25" t="inlineStr">
+      <c r="A61" s="38" t="inlineStr">
         <is>
           <t>3.2) Listar fabricantes dos módulos:</t>
         </is>
       </c>
-      <c r="B61" s="25" t="inlineStr">
-        <is>
-          <t>DAH SOLAR</t>
-        </is>
-      </c>
-      <c r="C61" s="25" t="n"/>
-      <c r="D61" s="22" t="n"/>
+      <c r="B61" s="38" t="inlineStr">
+        <is>
+          <t>ASTRONERGY</t>
+        </is>
+      </c>
+      <c r="C61" s="38" t="n"/>
+      <c r="D61" s="23" t="n"/>
       <c r="E61" s="40" t="n"/>
-      <c r="F61" s="24" t="n"/>
+      <c r="F61" s="37" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" s="25" t="inlineStr">
+      <c r="A62" s="38" t="inlineStr">
         <is>
           <t>3.3) Listar modelos dos módulos:</t>
         </is>
       </c>
-      <c r="B62" s="25" t="inlineStr">
+      <c r="B62" s="38" t="inlineStr">
         <is>
           <t>#MODMOD</t>
         </is>
       </c>
-      <c r="C62" s="25" t="n"/>
-      <c r="D62" s="22" t="n"/>
+      <c r="C62" s="38" t="n"/>
+      <c r="D62" s="23" t="n"/>
       <c r="E62" s="40" t="n"/>
-      <c r="F62" s="24" t="n"/>
+      <c r="F62" s="37" t="n"/>
     </row>
     <row r="63" ht="30" customHeight="1">
       <c r="A63" s="8" t="inlineStr">
@@ -1596,60 +1624,60 @@
           <t>3.4) Área total ocupada pelos arranjos (m2):</t>
         </is>
       </c>
-      <c r="B63" s="25" t="inlineStr">
+      <c r="B63" s="38" t="inlineStr">
         <is>
           <t>20.0</t>
         </is>
       </c>
-      <c r="C63" s="25" t="n"/>
-      <c r="D63" s="22" t="n"/>
+      <c r="C63" s="38" t="n"/>
+      <c r="D63" s="23" t="n"/>
       <c r="E63" s="40" t="n"/>
-      <c r="F63" s="24" t="n"/>
+      <c r="F63" s="37" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" s="25" t="inlineStr">
+      <c r="A64" s="38" t="inlineStr">
         <is>
           <t>3.5) Quantidade total de inversores:</t>
         </is>
       </c>
-      <c r="B64" s="25" t="inlineStr">
+      <c r="B64" s="38" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="C64" s="25" t="n"/>
-      <c r="D64" s="22" t="n"/>
+      <c r="C64" s="38" t="n"/>
+      <c r="D64" s="23" t="n"/>
       <c r="E64" s="40" t="n"/>
-      <c r="F64" s="24" t="n"/>
+      <c r="F64" s="37" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" s="25" t="inlineStr">
+      <c r="A65" s="38" t="inlineStr">
         <is>
           <t>3.6) Listar fabricantes dos inversores:</t>
         </is>
       </c>
-      <c r="B65" s="25" t="inlineStr">
+      <c r="B65" s="38" t="inlineStr">
         <is>
           <t>DEYE</t>
         </is>
       </c>
-      <c r="C65" s="25" t="n"/>
-      <c r="D65" s="22" t="n"/>
+      <c r="C65" s="38" t="n"/>
+      <c r="D65" s="23" t="n"/>
       <c r="E65" s="40" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" s="25" t="inlineStr">
+      <c r="A66" s="38" t="inlineStr">
         <is>
           <t>3.7) Listar modelos dos inversores:</t>
         </is>
       </c>
-      <c r="B66" s="25" t="inlineStr">
+      <c r="B66" s="38" t="inlineStr">
         <is>
           <t>SUN2000-G3-US-220</t>
         </is>
       </c>
-      <c r="C66" s="25" t="n"/>
-      <c r="D66" s="22" t="n"/>
+      <c r="C66" s="38" t="n"/>
+      <c r="D66" s="23" t="n"/>
       <c r="E66" s="40" t="n"/>
     </row>
     <row r="67" ht="45" customHeight="1">
@@ -1658,13 +1686,13 @@
           <t>3.8) Potência de pico dos módulos (soma das potências dos módulos, kWp): *</t>
         </is>
       </c>
-      <c r="B67" s="25" t="inlineStr">
-        <is>
-          <t>555.0</t>
-        </is>
-      </c>
-      <c r="C67" s="25" t="n"/>
-      <c r="D67" s="22" t="n"/>
+      <c r="B67" s="38" t="inlineStr">
+        <is>
+          <t>600.0</t>
+        </is>
+      </c>
+      <c r="C67" s="38" t="n"/>
+      <c r="D67" s="23" t="n"/>
       <c r="E67" s="40" t="n"/>
     </row>
     <row r="68" ht="45" customHeight="1">
@@ -1673,13 +1701,13 @@
           <t>3.9) Potência Nominal dos inversores (soma das potências nominais dos inversores, kW): *</t>
         </is>
       </c>
-      <c r="B68" s="25" t="inlineStr">
+      <c r="B68" s="38" t="inlineStr">
         <is>
           <t>2000.0</t>
         </is>
       </c>
-      <c r="C68" s="25" t="n"/>
-      <c r="D68" s="22" t="n"/>
+      <c r="C68" s="38" t="n"/>
+      <c r="D68" s="23" t="n"/>
       <c r="E68" s="40" t="n"/>
     </row>
     <row r="69" ht="30" customHeight="1">
@@ -1688,13 +1716,13 @@
           <t>3.10) Data pretendida para entrada em operação (dd/mm/aaaa):</t>
         </is>
       </c>
-      <c r="B69" s="25" t="inlineStr">
+      <c r="B69" s="38" t="inlineStr">
         <is>
           <t>05/06/2025</t>
         </is>
       </c>
-      <c r="C69" s="25" t="n"/>
-      <c r="D69" s="22" t="n"/>
+      <c r="C69" s="38" t="n"/>
+      <c r="D69" s="23" t="n"/>
       <c r="E69" s="40" t="n"/>
     </row>
     <row r="70">
@@ -1720,7 +1748,7 @@
           <t>Acréscimo</t>
         </is>
       </c>
-      <c r="D71" s="34" t="inlineStr">
+      <c r="D71" s="24" t="inlineStr">
         <is>
           <t>Total Previsto</t>
         </is>
@@ -1733,9 +1761,9 @@
           <t>4.1) Fabricante do aerogerador:</t>
         </is>
       </c>
-      <c r="B72" s="25" t="n"/>
-      <c r="C72" s="25" t="n"/>
-      <c r="D72" s="22" t="n"/>
+      <c r="B72" s="38" t="n"/>
+      <c r="C72" s="38" t="n"/>
+      <c r="D72" s="23" t="n"/>
       <c r="E72" s="40" t="n"/>
     </row>
     <row r="73">
@@ -1744,9 +1772,9 @@
           <t>4.2) Modelo do aerogerador:</t>
         </is>
       </c>
-      <c r="B73" s="25" t="n"/>
-      <c r="C73" s="25" t="n"/>
-      <c r="D73" s="22" t="n"/>
+      <c r="B73" s="38" t="n"/>
+      <c r="C73" s="38" t="n"/>
+      <c r="D73" s="23" t="n"/>
       <c r="E73" s="40" t="n"/>
     </row>
     <row r="74">
@@ -1755,9 +1783,9 @@
           <t>4.3) Eixo rotor (horizontal ou vertical):</t>
         </is>
       </c>
-      <c r="B74" s="25" t="n"/>
-      <c r="C74" s="25" t="n"/>
-      <c r="D74" s="22" t="n"/>
+      <c r="B74" s="38" t="n"/>
+      <c r="C74" s="38" t="n"/>
+      <c r="D74" s="23" t="n"/>
       <c r="E74" s="40" t="n"/>
     </row>
     <row r="75" ht="30" customHeight="1">
@@ -1766,9 +1794,9 @@
           <t>4.4) Altura máxima da pá ou atingida pela estrutura (m):</t>
         </is>
       </c>
-      <c r="B75" s="25" t="n"/>
-      <c r="C75" s="25" t="n"/>
-      <c r="D75" s="22" t="n"/>
+      <c r="B75" s="38" t="n"/>
+      <c r="C75" s="38" t="n"/>
+      <c r="D75" s="23" t="n"/>
       <c r="E75" s="40" t="n"/>
     </row>
     <row r="76" ht="30" customHeight="1">
@@ -1777,9 +1805,9 @@
           <t>4.5) Potência dos inversores (soma das potências dos inversores, kW): *</t>
         </is>
       </c>
-      <c r="B76" s="25" t="n"/>
-      <c r="C76" s="25" t="n"/>
-      <c r="D76" s="22" t="n"/>
+      <c r="B76" s="38" t="n"/>
+      <c r="C76" s="38" t="n"/>
+      <c r="D76" s="23" t="n"/>
       <c r="E76" s="40" t="n"/>
     </row>
     <row r="77" ht="45" customHeight="1">
@@ -1788,9 +1816,9 @@
           <t>4.6) Potência dos aerogeradores (soma potências dos aerogeradores, kW): *</t>
         </is>
       </c>
-      <c r="B77" s="25" t="n"/>
-      <c r="C77" s="25" t="n"/>
-      <c r="D77" s="22" t="n"/>
+      <c r="B77" s="38" t="n"/>
+      <c r="C77" s="38" t="n"/>
+      <c r="D77" s="23" t="n"/>
       <c r="E77" s="40" t="n"/>
     </row>
     <row r="78" ht="30" customHeight="1">
@@ -1799,9 +1827,9 @@
           <t>4.7) Data pretendida para entrada em operação (dd/mm/aaaa):</t>
         </is>
       </c>
-      <c r="B78" s="25" t="n"/>
-      <c r="C78" s="25" t="n"/>
-      <c r="D78" s="22" t="n"/>
+      <c r="B78" s="38" t="n"/>
+      <c r="C78" s="38" t="n"/>
+      <c r="D78" s="23" t="n"/>
       <c r="E78" s="40" t="n"/>
     </row>
     <row r="79" ht="30" customHeight="1">
@@ -1810,9 +1838,9 @@
           <t>4.8) Fabricante, modelo e tipo de conexão dos inversores:</t>
         </is>
       </c>
-      <c r="B79" s="25" t="n"/>
-      <c r="C79" s="25" t="n"/>
-      <c r="D79" s="22" t="n"/>
+      <c r="B79" s="38" t="n"/>
+      <c r="C79" s="38" t="n"/>
+      <c r="D79" s="23" t="n"/>
       <c r="E79" s="40" t="n"/>
     </row>
     <row r="80">
@@ -1821,9 +1849,9 @@
           <t>4.9) Quantidade de inversores: *</t>
         </is>
       </c>
-      <c r="B80" s="25" t="n"/>
-      <c r="C80" s="25" t="n"/>
-      <c r="D80" s="22" t="n"/>
+      <c r="B80" s="38" t="n"/>
+      <c r="C80" s="38" t="n"/>
+      <c r="D80" s="23" t="n"/>
       <c r="E80" s="40" t="n"/>
     </row>
     <row r="81" ht="30" customHeight="1">
@@ -1832,9 +1860,9 @@
           <t>4.10) Potência (soma das potências nominais dos inversores, kW): *</t>
         </is>
       </c>
-      <c r="B81" s="25" t="n"/>
-      <c r="C81" s="25" t="n"/>
-      <c r="D81" s="22" t="n"/>
+      <c r="B81" s="38" t="n"/>
+      <c r="C81" s="38" t="n"/>
+      <c r="D81" s="23" t="n"/>
       <c r="E81" s="40" t="n"/>
     </row>
     <row r="82">
@@ -1860,7 +1888,7 @@
           <t>Acréscimo</t>
         </is>
       </c>
-      <c r="D83" s="34" t="inlineStr">
+      <c r="D83" s="24" t="inlineStr">
         <is>
           <t>Total Previsto</t>
         </is>
@@ -1873,9 +1901,9 @@
           <t>5.1) Rio onde se localiza a central geradora:</t>
         </is>
       </c>
-      <c r="B84" s="25" t="n"/>
-      <c r="C84" s="25" t="n"/>
-      <c r="D84" s="22" t="n"/>
+      <c r="B84" s="38" t="n"/>
+      <c r="C84" s="38" t="n"/>
+      <c r="D84" s="23" t="n"/>
       <c r="E84" s="40" t="n"/>
     </row>
     <row r="85">
@@ -1884,9 +1912,9 @@
           <t>5.2) Bacia onde se localiza o rio:</t>
         </is>
       </c>
-      <c r="B85" s="25" t="n"/>
-      <c r="C85" s="25" t="n"/>
-      <c r="D85" s="22" t="n"/>
+      <c r="B85" s="38" t="n"/>
+      <c r="C85" s="38" t="n"/>
+      <c r="D85" s="23" t="n"/>
       <c r="E85" s="40" t="n"/>
     </row>
     <row r="86">
@@ -1895,9 +1923,9 @@
           <t>5.3) Sub-bacia onde se localiza o rio:</t>
         </is>
       </c>
-      <c r="B86" s="25" t="n"/>
-      <c r="C86" s="25" t="n"/>
-      <c r="D86" s="22" t="n"/>
+      <c r="B86" s="38" t="n"/>
+      <c r="C86" s="38" t="n"/>
+      <c r="D86" s="23" t="n"/>
       <c r="E86" s="40" t="n"/>
     </row>
     <row r="87">
@@ -1906,9 +1934,9 @@
           <t>5.4) Tipo de turbina: *</t>
         </is>
       </c>
-      <c r="B87" s="25" t="n"/>
-      <c r="C87" s="25" t="n"/>
-      <c r="D87" s="22" t="n"/>
+      <c r="B87" s="38" t="n"/>
+      <c r="C87" s="38" t="n"/>
+      <c r="D87" s="23" t="n"/>
       <c r="E87" s="40" t="n"/>
     </row>
     <row r="88" ht="45" customHeight="1">
@@ -1917,9 +1945,9 @@
           <t>5.5) Potência turbina (soma potências nominais das turbinas, kVA): *</t>
         </is>
       </c>
-      <c r="B88" s="25" t="n"/>
-      <c r="C88" s="25" t="n"/>
-      <c r="D88" s="22" t="n"/>
+      <c r="B88" s="38" t="n"/>
+      <c r="C88" s="38" t="n"/>
+      <c r="D88" s="23" t="n"/>
       <c r="E88" s="40" t="n"/>
     </row>
     <row r="89" ht="45" customHeight="1">
@@ -1928,9 +1956,9 @@
           <t>5.6) Potência gerador (soma potências nominais dos geradores, kVA): *</t>
         </is>
       </c>
-      <c r="B89" s="25" t="n"/>
-      <c r="C89" s="25" t="n"/>
-      <c r="D89" s="22" t="n"/>
+      <c r="B89" s="38" t="n"/>
+      <c r="C89" s="38" t="n"/>
+      <c r="D89" s="23" t="n"/>
       <c r="E89" s="40" t="n"/>
     </row>
     <row r="90" ht="30" customHeight="1">
@@ -1939,9 +1967,9 @@
           <t>5.7) Fator de potência do gerador (entre 0 e 1): *</t>
         </is>
       </c>
-      <c r="B90" s="25" t="n"/>
-      <c r="C90" s="25" t="n"/>
-      <c r="D90" s="22" t="n"/>
+      <c r="B90" s="38" t="n"/>
+      <c r="C90" s="38" t="n"/>
+      <c r="D90" s="23" t="n"/>
       <c r="E90" s="40" t="n"/>
     </row>
     <row r="91">
@@ -1950,9 +1978,9 @@
           <t>5.8) Potência ativa do gerador (kW): *</t>
         </is>
       </c>
-      <c r="B91" s="25" t="n"/>
-      <c r="C91" s="25" t="n"/>
-      <c r="D91" s="22" t="n"/>
+      <c r="B91" s="38" t="n"/>
+      <c r="C91" s="38" t="n"/>
+      <c r="D91" s="23" t="n"/>
       <c r="E91" s="40" t="n"/>
     </row>
     <row r="92" ht="30" customHeight="1">
@@ -1961,9 +1989,9 @@
           <t>5.9) Potência aparente do gerador (kVA): *</t>
         </is>
       </c>
-      <c r="B92" s="25" t="n"/>
-      <c r="C92" s="25" t="n"/>
-      <c r="D92" s="22" t="n"/>
+      <c r="B92" s="38" t="n"/>
+      <c r="C92" s="38" t="n"/>
+      <c r="D92" s="23" t="n"/>
       <c r="E92" s="40" t="n"/>
     </row>
     <row r="93">
@@ -1972,9 +2000,9 @@
           <t>5.10) Tensão (kV):</t>
         </is>
       </c>
-      <c r="B93" s="25" t="n"/>
-      <c r="C93" s="25" t="n"/>
-      <c r="D93" s="22" t="n"/>
+      <c r="B93" s="38" t="n"/>
+      <c r="C93" s="38" t="n"/>
+      <c r="D93" s="23" t="n"/>
       <c r="E93" s="40" t="n"/>
     </row>
     <row r="94" ht="30" customHeight="1">
@@ -1983,9 +2011,9 @@
           <t>5.11) Nível Operacional Normal de Montante (m)</t>
         </is>
       </c>
-      <c r="B94" s="25" t="n"/>
-      <c r="C94" s="25" t="n"/>
-      <c r="D94" s="22" t="n"/>
+      <c r="B94" s="38" t="n"/>
+      <c r="C94" s="38" t="n"/>
+      <c r="D94" s="23" t="n"/>
       <c r="E94" s="40" t="n"/>
     </row>
     <row r="95" ht="30" customHeight="1">
@@ -1994,9 +2022,9 @@
           <t>5.12) Nível Operacional Normal de Jusante (m)</t>
         </is>
       </c>
-      <c r="B95" s="25" t="n"/>
-      <c r="C95" s="25" t="n"/>
-      <c r="D95" s="22" t="n"/>
+      <c r="B95" s="38" t="n"/>
+      <c r="C95" s="38" t="n"/>
+      <c r="D95" s="23" t="n"/>
       <c r="E95" s="40" t="n"/>
     </row>
     <row r="96" ht="30" customHeight="1">
@@ -2005,9 +2033,9 @@
           <t>5.13) Data pretendida para entrada em operação (dd/mm/aaaa):</t>
         </is>
       </c>
-      <c r="B96" s="25" t="n"/>
-      <c r="C96" s="25" t="n"/>
-      <c r="D96" s="22" t="n"/>
+      <c r="B96" s="38" t="n"/>
+      <c r="C96" s="38" t="n"/>
+      <c r="D96" s="23" t="n"/>
       <c r="E96" s="40" t="n"/>
     </row>
     <row r="97" ht="30" customHeight="1">
@@ -2016,9 +2044,9 @@
           <t>5.14) Fabricante, modelo e tipo de conexão dos inversores:</t>
         </is>
       </c>
-      <c r="B97" s="25" t="n"/>
-      <c r="C97" s="25" t="n"/>
-      <c r="D97" s="22" t="n"/>
+      <c r="B97" s="38" t="n"/>
+      <c r="C97" s="38" t="n"/>
+      <c r="D97" s="23" t="n"/>
       <c r="E97" s="40" t="n"/>
     </row>
     <row r="98">
@@ -2027,9 +2055,9 @@
           <t>5.15) Quantidade de inversores: *</t>
         </is>
       </c>
-      <c r="B98" s="25" t="n"/>
-      <c r="C98" s="25" t="n"/>
-      <c r="D98" s="22" t="n"/>
+      <c r="B98" s="38" t="n"/>
+      <c r="C98" s="38" t="n"/>
+      <c r="D98" s="23" t="n"/>
       <c r="E98" s="40" t="n"/>
     </row>
     <row r="99" ht="30" customHeight="1">
@@ -2038,9 +2066,9 @@
           <t>5.16) Potência (soma das potências nominais dos inversores, kW): *</t>
         </is>
       </c>
-      <c r="B99" s="25" t="n"/>
-      <c r="C99" s="25" t="n"/>
-      <c r="D99" s="22" t="n"/>
+      <c r="B99" s="38" t="n"/>
+      <c r="C99" s="38" t="n"/>
+      <c r="D99" s="23" t="n"/>
       <c r="E99" s="40" t="n"/>
     </row>
     <row r="100">
@@ -2066,7 +2094,7 @@
           <t>Acréscimo</t>
         </is>
       </c>
-      <c r="D101" s="34" t="inlineStr">
+      <c r="D101" s="24" t="inlineStr">
         <is>
           <t>Total Previsto</t>
         </is>
@@ -2079,11 +2107,11 @@
           <t>6.1) Fabricante e modelo:</t>
         </is>
       </c>
-      <c r="B102" s="25" t="n"/>
-      <c r="C102" s="25" t="n"/>
-      <c r="D102" s="22" t="inlineStr">
-        <is>
-          <t>DAH SOLAR , #MODMOD</t>
+      <c r="B102" s="38" t="n"/>
+      <c r="C102" s="38" t="n"/>
+      <c r="D102" s="23" t="inlineStr">
+        <is>
+          <t>ASTRONERGY , #MODMOD</t>
         </is>
       </c>
       <c r="E102" s="40" t="n"/>
@@ -2094,11 +2122,11 @@
           <t>6.2) Potência (soma das potências nominais dos geradores, kVA): *</t>
         </is>
       </c>
-      <c r="B103" s="25" t="n"/>
-      <c r="C103" s="25" t="n"/>
-      <c r="D103" s="22" t="inlineStr">
-        <is>
-          <t>555.0</t>
+      <c r="B103" s="38" t="n"/>
+      <c r="C103" s="38" t="n"/>
+      <c r="D103" s="23" t="inlineStr">
+        <is>
+          <t>600.0</t>
         </is>
       </c>
       <c r="E103" s="40" t="n"/>
@@ -2109,9 +2137,9 @@
           <t>6.3) Fator de potência (entre 0 e 1): *</t>
         </is>
       </c>
-      <c r="B104" s="25" t="n"/>
-      <c r="C104" s="25" t="n"/>
-      <c r="D104" s="22" t="n">
+      <c r="B104" s="38" t="n"/>
+      <c r="C104" s="38" t="n"/>
+      <c r="D104" s="23" t="n">
         <v>1</v>
       </c>
       <c r="E104" s="40" t="n"/>
@@ -2122,9 +2150,9 @@
           <t>6.4) Potência ativa (kW): *</t>
         </is>
       </c>
-      <c r="B105" s="25" t="n"/>
-      <c r="C105" s="25" t="n"/>
-      <c r="D105" s="22" t="inlineStr">
+      <c r="B105" s="38" t="n"/>
+      <c r="C105" s="38" t="n"/>
+      <c r="D105" s="23" t="inlineStr">
         <is>
           <t>4.0</t>
         </is>
@@ -2137,9 +2165,9 @@
           <t>6.5) Fonte (indicar segundo lista do Item 7 a seguir, conforme aplicável): *</t>
         </is>
       </c>
-      <c r="B106" s="25" t="n"/>
-      <c r="C106" s="25" t="n"/>
-      <c r="D106" s="22" t="inlineStr">
+      <c r="B106" s="38" t="n"/>
+      <c r="C106" s="38" t="n"/>
+      <c r="D106" s="23" t="inlineStr">
         <is>
           <t>7.6</t>
         </is>
@@ -2152,9 +2180,9 @@
           <t>6.6) Data pretendida para entrada em operação (dd/mm/aaaa):</t>
         </is>
       </c>
-      <c r="B107" s="25" t="n"/>
-      <c r="C107" s="25" t="n"/>
-      <c r="D107" s="22" t="inlineStr">
+      <c r="B107" s="38" t="n"/>
+      <c r="C107" s="38" t="n"/>
+      <c r="D107" s="23" t="inlineStr">
         <is>
           <t>05/06/2025</t>
         </is>
@@ -2167,9 +2195,9 @@
           <t>6.7) Ciclo (aberto/fechado): *</t>
         </is>
       </c>
-      <c r="B108" s="25" t="n"/>
-      <c r="C108" s="25" t="n"/>
-      <c r="D108" s="22" t="n"/>
+      <c r="B108" s="38" t="n"/>
+      <c r="C108" s="38" t="n"/>
+      <c r="D108" s="23" t="n"/>
       <c r="E108" s="40" t="n"/>
     </row>
     <row r="109">
@@ -2178,9 +2206,9 @@
           <t>6.8) Máquina Motriz: *</t>
         </is>
       </c>
-      <c r="B109" s="25" t="n"/>
-      <c r="C109" s="25" t="n"/>
-      <c r="D109" s="22" t="n"/>
+      <c r="B109" s="38" t="n"/>
+      <c r="C109" s="38" t="n"/>
+      <c r="D109" s="23" t="n"/>
       <c r="E109" s="40" t="n"/>
     </row>
     <row r="110" ht="30" customHeight="1">
@@ -2189,9 +2217,9 @@
           <t>6.9) Número do Despacho de qualificação como cogeradora: *</t>
         </is>
       </c>
-      <c r="B110" s="25" t="n"/>
-      <c r="C110" s="25" t="n"/>
-      <c r="D110" s="22" t="n"/>
+      <c r="B110" s="38" t="n"/>
+      <c r="C110" s="38" t="n"/>
+      <c r="D110" s="23" t="n"/>
       <c r="E110" s="40" t="n"/>
     </row>
     <row r="111">
@@ -2200,9 +2228,9 @@
           <t>6.10) Data do Despacho: *</t>
         </is>
       </c>
-      <c r="B111" s="25" t="n"/>
-      <c r="C111" s="25" t="n"/>
-      <c r="D111" s="22" t="n"/>
+      <c r="B111" s="38" t="n"/>
+      <c r="C111" s="38" t="n"/>
+      <c r="D111" s="23" t="n"/>
       <c r="E111" s="40" t="n"/>
     </row>
     <row r="112" ht="30" customHeight="1">
@@ -2211,9 +2239,9 @@
           <t>6.11) Tensão Terminal Nominal (Vn kV)</t>
         </is>
       </c>
-      <c r="B112" s="25" t="n"/>
-      <c r="C112" s="25" t="n"/>
-      <c r="D112" s="22" t="n"/>
+      <c r="B112" s="38" t="n"/>
+      <c r="C112" s="38" t="n"/>
+      <c r="D112" s="23" t="n"/>
       <c r="E112" s="40" t="n"/>
     </row>
     <row r="113" ht="30" customHeight="1">
@@ -2222,9 +2250,9 @@
           <t>6.12) Reatância síncrona de eixo direto (Xd, em pu)</t>
         </is>
       </c>
-      <c r="B113" s="25" t="n"/>
-      <c r="C113" s="25" t="n"/>
-      <c r="D113" s="22" t="n"/>
+      <c r="B113" s="38" t="n"/>
+      <c r="C113" s="38" t="n"/>
+      <c r="D113" s="23" t="n"/>
       <c r="E113" s="40" t="n"/>
     </row>
     <row r="114" ht="30" customHeight="1">
@@ -2233,9 +2261,9 @@
           <t>6.13) Reatância transitória de eixo direto (Xd’, em pu)</t>
         </is>
       </c>
-      <c r="B114" s="25" t="n"/>
-      <c r="C114" s="25" t="n"/>
-      <c r="D114" s="22" t="n"/>
+      <c r="B114" s="38" t="n"/>
+      <c r="C114" s="38" t="n"/>
+      <c r="D114" s="23" t="n"/>
       <c r="E114" s="40" t="n"/>
     </row>
     <row r="115" ht="30" customHeight="1">
@@ -2244,9 +2272,9 @@
           <t>6.14) Reatância sub-transitória de eixo direto (Xd’’, em pu)</t>
         </is>
       </c>
-      <c r="B115" s="25" t="n"/>
-      <c r="C115" s="25" t="n"/>
-      <c r="D115" s="22" t="n"/>
+      <c r="B115" s="38" t="n"/>
+      <c r="C115" s="38" t="n"/>
+      <c r="D115" s="23" t="n"/>
       <c r="E115" s="40" t="n"/>
     </row>
     <row r="116" ht="30" customHeight="1">
@@ -2255,9 +2283,9 @@
           <t>6.15) Reatância de sequência negativa (X2, em pu)</t>
         </is>
       </c>
-      <c r="B116" s="25" t="n"/>
-      <c r="C116" s="25" t="n"/>
-      <c r="D116" s="22" t="n"/>
+      <c r="B116" s="38" t="n"/>
+      <c r="C116" s="38" t="n"/>
+      <c r="D116" s="23" t="n"/>
       <c r="E116" s="40" t="n"/>
     </row>
     <row r="117" ht="30" customHeight="1">
@@ -2266,9 +2294,9 @@
           <t>6.16) Reatância de sequência zero (X0, em pu)</t>
         </is>
       </c>
-      <c r="B117" s="25" t="n"/>
-      <c r="C117" s="25" t="n"/>
-      <c r="D117" s="22" t="n"/>
+      <c r="B117" s="38" t="n"/>
+      <c r="C117" s="38" t="n"/>
+      <c r="D117" s="23" t="n"/>
       <c r="E117" s="40" t="n"/>
     </row>
     <row r="118" ht="30" customHeight="1">
@@ -2277,9 +2305,9 @@
           <t>6.17) Reatância síncrona de eixo em quadratura (Xq, em pu)</t>
         </is>
       </c>
-      <c r="B118" s="25" t="n"/>
-      <c r="C118" s="25" t="n"/>
-      <c r="D118" s="22" t="n"/>
+      <c r="B118" s="38" t="n"/>
+      <c r="C118" s="38" t="n"/>
+      <c r="D118" s="23" t="n"/>
       <c r="E118" s="40" t="n"/>
     </row>
     <row r="119" ht="30" customHeight="1">
@@ -2288,9 +2316,9 @@
           <t>6.18) Resistência do enrolamento de armadura (Ra, em pu)</t>
         </is>
       </c>
-      <c r="B119" s="25" t="n"/>
-      <c r="C119" s="25" t="n"/>
-      <c r="D119" s="22" t="n"/>
+      <c r="B119" s="38" t="n"/>
+      <c r="C119" s="38" t="n"/>
+      <c r="D119" s="23" t="n"/>
       <c r="E119" s="40" t="n"/>
     </row>
     <row r="120" ht="30" customHeight="1">
@@ -2299,9 +2327,9 @@
           <t>6.19) Constante de inércia, em segundos (H)</t>
         </is>
       </c>
-      <c r="B120" s="25" t="n"/>
-      <c r="C120" s="25" t="n"/>
-      <c r="D120" s="22" t="n"/>
+      <c r="B120" s="38" t="n"/>
+      <c r="C120" s="38" t="n"/>
+      <c r="D120" s="23" t="n"/>
       <c r="E120" s="40" t="n"/>
     </row>
     <row r="121" ht="30" customHeight="1">
@@ -2310,9 +2338,9 @@
           <t>6.20) Constante de amortecimento, em pu/pu. (D)</t>
         </is>
       </c>
-      <c r="B121" s="25" t="n"/>
-      <c r="C121" s="25" t="n"/>
-      <c r="D121" s="22" t="n"/>
+      <c r="B121" s="38" t="n"/>
+      <c r="C121" s="38" t="n"/>
+      <c r="D121" s="23" t="n"/>
       <c r="E121" s="40" t="n"/>
     </row>
     <row r="122" ht="30" customHeight="1">
@@ -2321,9 +2349,9 @@
           <t>6.21) Fabricante, modelo e tipo de conexão dos inversores:</t>
         </is>
       </c>
-      <c r="B122" s="25" t="n"/>
-      <c r="C122" s="25" t="n"/>
-      <c r="D122" s="22" t="inlineStr">
+      <c r="B122" s="38" t="n"/>
+      <c r="C122" s="38" t="n"/>
+      <c r="D122" s="23" t="inlineStr">
         <is>
           <t>DEYE , SUN2000-G3-US-220</t>
         </is>
@@ -2336,9 +2364,9 @@
           <t>6.22) Quantidade de inversores: *</t>
         </is>
       </c>
-      <c r="B123" s="25" t="n"/>
-      <c r="C123" s="25" t="n"/>
-      <c r="D123" s="22" t="inlineStr">
+      <c r="B123" s="38" t="n"/>
+      <c r="C123" s="38" t="n"/>
+      <c r="D123" s="23" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -2351,9 +2379,9 @@
           <t>6.23) Potência (soma das potências nominais dos inversores, kW): *</t>
         </is>
       </c>
-      <c r="B124" s="25" t="n"/>
-      <c r="C124" s="25" t="n"/>
-      <c r="D124" s="22" t="inlineStr">
+      <c r="B124" s="38" t="n"/>
+      <c r="C124" s="38" t="n"/>
+      <c r="D124" s="23" t="inlineStr">
         <is>
           <t>2000.0</t>
         </is>
@@ -2368,7 +2396,7 @@
       <c r="E125" s="40" t="n"/>
     </row>
     <row r="126">
-      <c r="A126" s="30" t="inlineStr">
+      <c r="A126" s="22" t="inlineStr">
         <is>
           <t>7) Fontes Primárias de Energia da Central Geradora Elétrica (para preenchimento do item 6.5)</t>
         </is>
@@ -2379,7 +2407,7 @@
       <c r="E126" s="40" t="n"/>
     </row>
     <row r="127">
-      <c r="A127" s="29" t="inlineStr">
+      <c r="A127" s="33" t="inlineStr">
         <is>
           <t>7.1) Origem em biomassa (floresta, resíduos sólidos, resíduos animais, biocombustíveis líquidos, agroindustriais)</t>
         </is>
@@ -2390,7 +2418,7 @@
       <c r="E127" s="40" t="n"/>
     </row>
     <row r="128">
-      <c r="A128" s="28" t="inlineStr">
+      <c r="A128" s="32" t="inlineStr">
         <is>
           <t>Biogás (floresta)</t>
         </is>
@@ -2401,7 +2429,7 @@
       <c r="E128" s="40" t="n"/>
     </row>
     <row r="129">
-      <c r="A129" s="28" t="inlineStr">
+      <c r="A129" s="32" t="inlineStr">
         <is>
           <t>Biogás (resíduo sólido urbano, RU)</t>
         </is>
@@ -2412,7 +2440,7 @@
       <c r="E129" s="40" t="n"/>
     </row>
     <row r="130">
-      <c r="A130" s="28" t="inlineStr">
+      <c r="A130" s="32" t="inlineStr">
         <is>
           <t>Biogás (resíduo animal, RA)</t>
         </is>
@@ -2423,7 +2451,7 @@
       <c r="E130" s="40" t="n"/>
     </row>
     <row r="131">
-      <c r="A131" s="28" t="inlineStr">
+      <c r="A131" s="32" t="inlineStr">
         <is>
           <t>Biogás (agroindustrial)</t>
         </is>
@@ -2434,7 +2462,7 @@
       <c r="E131" s="40" t="n"/>
     </row>
     <row r="132">
-      <c r="A132" s="28" t="inlineStr">
+      <c r="A132" s="32" t="inlineStr">
         <is>
           <t>Carvão vegetal</t>
         </is>
@@ -2445,7 +2473,7 @@
       <c r="E132" s="40" t="n"/>
     </row>
     <row r="133">
-      <c r="A133" s="28" t="inlineStr">
+      <c r="A133" s="32" t="inlineStr">
         <is>
           <t>Gás de alto-forno (de biomassa)</t>
         </is>
@@ -2456,7 +2484,7 @@
       <c r="E133" s="40" t="n"/>
     </row>
     <row r="134">
-      <c r="A134" s="28" t="inlineStr">
+      <c r="A134" s="32" t="inlineStr">
         <is>
           <t>Lenha</t>
         </is>
@@ -2467,7 +2495,7 @@
       <c r="E134" s="40" t="n"/>
     </row>
     <row r="135">
-      <c r="A135" s="28" t="inlineStr">
+      <c r="A135" s="32" t="inlineStr">
         <is>
           <t>Licor negro</t>
         </is>
@@ -2478,7 +2506,7 @@
       <c r="E135" s="40" t="n"/>
     </row>
     <row r="136">
-      <c r="A136" s="28" t="inlineStr">
+      <c r="A136" s="32" t="inlineStr">
         <is>
           <t>Resíduos de madeira</t>
         </is>
@@ -2489,7 +2517,7 @@
       <c r="E136" s="40" t="n"/>
     </row>
     <row r="137">
-      <c r="A137" s="28" t="inlineStr">
+      <c r="A137" s="32" t="inlineStr">
         <is>
           <t>Etanol</t>
         </is>
@@ -2500,7 +2528,7 @@
       <c r="E137" s="40" t="n"/>
     </row>
     <row r="138">
-      <c r="A138" s="28" t="inlineStr">
+      <c r="A138" s="32" t="inlineStr">
         <is>
           <t>Óleos vegetais</t>
         </is>
@@ -2511,7 +2539,7 @@
       <c r="E138" s="40" t="n"/>
     </row>
     <row r="139">
-      <c r="A139" s="28" t="inlineStr">
+      <c r="A139" s="32" t="inlineStr">
         <is>
           <t>Bagaço de cana-de-açúcar</t>
         </is>
@@ -2522,7 +2550,7 @@
       <c r="E139" s="40" t="n"/>
     </row>
     <row r="140">
-      <c r="A140" s="28" t="inlineStr">
+      <c r="A140" s="32" t="inlineStr">
         <is>
           <t>Capim elefante</t>
         </is>
@@ -2533,7 +2561,7 @@
       <c r="E140" s="40" t="n"/>
     </row>
     <row r="141">
-      <c r="A141" s="28" t="inlineStr">
+      <c r="A141" s="32" t="inlineStr">
         <is>
           <t>Casca de arroz</t>
         </is>
@@ -2544,7 +2572,7 @@
       <c r="E141" s="40" t="n"/>
     </row>
     <row r="142">
-      <c r="A142" s="29" t="inlineStr">
+      <c r="A142" s="33" t="inlineStr">
         <is>
           <t>7.2) Eólica (cinética do vento):</t>
         </is>
@@ -2555,7 +2583,7 @@
       <c r="E142" s="40" t="n"/>
     </row>
     <row r="143">
-      <c r="A143" s="29" t="inlineStr">
+      <c r="A143" s="33" t="inlineStr">
         <is>
           <t>7.3) Fóssil (petróleo, carvão mineral, gás natural, outros):</t>
         </is>
@@ -2566,7 +2594,7 @@
       <c r="E143" s="40" t="n"/>
     </row>
     <row r="144">
-      <c r="A144" s="28" t="inlineStr">
+      <c r="A144" s="32" t="inlineStr">
         <is>
           <t>Gás de alto-forno (de petróleo)</t>
         </is>
@@ -2577,7 +2605,7 @@
       <c r="E144" s="40" t="n"/>
     </row>
     <row r="145">
-      <c r="A145" s="28" t="inlineStr">
+      <c r="A145" s="32" t="inlineStr">
         <is>
           <t>Gás de refinaria (de petróleo)</t>
         </is>
@@ -2588,7 +2616,7 @@
       <c r="E145" s="40" t="n"/>
     </row>
     <row r="146">
-      <c r="A146" s="28" t="inlineStr">
+      <c r="A146" s="32" t="inlineStr">
         <is>
           <t>Óleo combustível</t>
         </is>
@@ -2599,7 +2627,7 @@
       <c r="E146" s="40" t="n"/>
     </row>
     <row r="147">
-      <c r="A147" s="28" t="inlineStr">
+      <c r="A147" s="32" t="inlineStr">
         <is>
           <t>Óleo diesel</t>
         </is>
@@ -2610,7 +2638,7 @@
       <c r="E147" s="40" t="n"/>
     </row>
     <row r="148">
-      <c r="A148" s="28" t="inlineStr">
+      <c r="A148" s="32" t="inlineStr">
         <is>
           <t>Outros energéticos de petróleo</t>
         </is>
@@ -2621,7 +2649,7 @@
       <c r="E148" s="40" t="n"/>
     </row>
     <row r="149">
-      <c r="A149" s="28" t="inlineStr">
+      <c r="A149" s="32" t="inlineStr">
         <is>
           <t>Carvão mineral</t>
         </is>
@@ -2632,7 +2660,7 @@
       <c r="E149" s="40" t="n"/>
     </row>
     <row r="150">
-      <c r="A150" s="28" t="inlineStr">
+      <c r="A150" s="32" t="inlineStr">
         <is>
           <t>Calor de processo (de carvão mineral)</t>
         </is>
@@ -2643,7 +2671,7 @@
       <c r="E150" s="40" t="n"/>
     </row>
     <row r="151">
-      <c r="A151" s="28" t="inlineStr">
+      <c r="A151" s="32" t="inlineStr">
         <is>
           <t>Gás de alto-forno (de carvão mineral)</t>
         </is>
@@ -2654,7 +2682,7 @@
       <c r="E151" s="40" t="n"/>
     </row>
     <row r="152">
-      <c r="A152" s="28" t="inlineStr">
+      <c r="A152" s="32" t="inlineStr">
         <is>
           <t>Gás natural</t>
         </is>
@@ -2665,7 +2693,7 @@
       <c r="E152" s="40" t="n"/>
     </row>
     <row r="153">
-      <c r="A153" s="28" t="inlineStr">
+      <c r="A153" s="32" t="inlineStr">
         <is>
           <t>Calor de processo (de gás natural)</t>
         </is>
@@ -2676,7 +2704,7 @@
       <c r="E153" s="40" t="n"/>
     </row>
     <row r="154">
-      <c r="A154" s="28" t="inlineStr">
+      <c r="A154" s="32" t="inlineStr">
         <is>
           <t>Calor de processo (de outras fontes fósseis)</t>
         </is>
@@ -2687,7 +2715,7 @@
       <c r="E154" s="40" t="n"/>
     </row>
     <row r="155">
-      <c r="A155" s="28" t="inlineStr">
+      <c r="A155" s="32" t="inlineStr">
         <is>
           <t>Turfa</t>
         </is>
@@ -2698,7 +2726,7 @@
       <c r="E155" s="40" t="n"/>
     </row>
     <row r="156">
-      <c r="A156" s="28" t="inlineStr">
+      <c r="A156" s="32" t="inlineStr">
         <is>
           <t>Xisto</t>
         </is>
@@ -2709,7 +2737,7 @@
       <c r="E156" s="40" t="n"/>
     </row>
     <row r="157">
-      <c r="A157" s="25" t="inlineStr">
+      <c r="A157" s="38" t="inlineStr">
         <is>
           <t>7.4) Hídrica (potencial hidráulico)</t>
         </is>
@@ -2720,7 +2748,7 @@
       <c r="E157" s="40" t="n"/>
     </row>
     <row r="158">
-      <c r="A158" s="25" t="inlineStr">
+      <c r="A158" s="38" t="inlineStr">
         <is>
           <t>7.5) Nuclear (urânio)</t>
         </is>
@@ -2731,7 +2759,7 @@
       <c r="E158" s="40" t="n"/>
     </row>
     <row r="159">
-      <c r="A159" s="25" t="inlineStr">
+      <c r="A159" s="38" t="inlineStr">
         <is>
           <t>7.6) Solar (radiação solar)</t>
         </is>
@@ -2742,7 +2770,7 @@
       <c r="E159" s="40" t="n"/>
     </row>
     <row r="160">
-      <c r="A160" s="25" t="inlineStr">
+      <c r="A160" s="38" t="inlineStr">
         <is>
           <t>7.7) Undi-elétrica (cinética da água)</t>
         </is>
@@ -2755,19 +2783,19 @@
   </sheetData>
   <sheetProtection selectLockedCells="0" selectUnlockedCells="0" algorithmName="SHA-512" sheet="1" objects="1" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="1" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" saltValue="0cHIyALx0C5q/DQCNrXsAw==" formatRows="1" sort="1" spinCount="100000" hashValue="RiMd7wkIqV2kKc8BpI75WcH1nWOoXpFZuiKwZG0pksFxhmRb/TowVssgMWoEcciBiOD46ygwxtJTs3eoppNgXA=="/>
   <mergeCells count="161">
+    <mergeCell ref="A39:E39"/>
     <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A39:E39"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="F33:H33"/>
     <mergeCell ref="A142:E142"/>
     <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D84:E84"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="D84:E84"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="B36:E36"/>
+    <mergeCell ref="D77:E77"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D77:E77"/>
     <mergeCell ref="D108:E108"/>
     <mergeCell ref="D86:E86"/>
     <mergeCell ref="A128:E128"/>
@@ -2776,9 +2804,9 @@
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="A136:E136"/>
     <mergeCell ref="A139:E139"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="D78:E78"/>
     <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F14:H14"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="D112:E112"/>
     <mergeCell ref="A129:E129"/>
@@ -2787,16 +2815,16 @@
     <mergeCell ref="D71:E71"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="D114:E114"/>
+    <mergeCell ref="A131:E131"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A131:E131"/>
     <mergeCell ref="A100:E100"/>
+    <mergeCell ref="A156:E156"/>
     <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A156:E156"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D73:E73"/>
     <mergeCell ref="B13:E13"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D98:E98"/>
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="D113:E113"/>
@@ -2811,8 +2839,8 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A138:E138"/>
     <mergeCell ref="D99:E99"/>
-    <mergeCell ref="A138:E138"/>
     <mergeCell ref="A132:E132"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D101:E101"/>
@@ -2823,8 +2851,8 @@
     <mergeCell ref="A133:E133"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D53:E53"/>
     <mergeCell ref="A3:E3"/>
-    <mergeCell ref="D53:E53"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="D103:E103"/>
     <mergeCell ref="B11:E11"/>
@@ -2836,20 +2864,20 @@
     <mergeCell ref="D89:E89"/>
     <mergeCell ref="B37:E37"/>
     <mergeCell ref="D79:E79"/>
+    <mergeCell ref="A82:E82"/>
     <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A82:E82"/>
     <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F32:H32"/>
     <mergeCell ref="D81:E81"/>
-    <mergeCell ref="F32:H32"/>
     <mergeCell ref="B15:E15"/>
+    <mergeCell ref="D96:E96"/>
     <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D96:E96"/>
     <mergeCell ref="A146:E146"/>
     <mergeCell ref="D105:E105"/>
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D120:E120"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D120:E120"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="D107:E107"/>
     <mergeCell ref="D116:E116"/>
@@ -2860,13 +2888,13 @@
     <mergeCell ref="A151:E151"/>
     <mergeCell ref="A160:E160"/>
     <mergeCell ref="D93:E93"/>
+    <mergeCell ref="A141:E141"/>
     <mergeCell ref="D102:E102"/>
-    <mergeCell ref="A141:E141"/>
     <mergeCell ref="A135:E135"/>
     <mergeCell ref="A150:E150"/>
     <mergeCell ref="A144:E144"/>
+    <mergeCell ref="D83:E83"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D83:E83"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="D117:E117"/>
     <mergeCell ref="D92:E92"/>
@@ -2874,9 +2902,9 @@
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="A125:E125"/>
     <mergeCell ref="A134:E134"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="A28:E28"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="D67:E67"/>
     <mergeCell ref="A152:E152"/>
     <mergeCell ref="D85:E85"/>
     <mergeCell ref="D54:E54"/>
@@ -2887,11 +2915,11 @@
     <mergeCell ref="D109:E109"/>
     <mergeCell ref="D119:E119"/>
     <mergeCell ref="B5:E5"/>
+    <mergeCell ref="D111:E111"/>
     <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D111:E111"/>
     <mergeCell ref="A70:E70"/>
+    <mergeCell ref="A153:E153"/>
     <mergeCell ref="D21:E21"/>
-    <mergeCell ref="A153:E153"/>
     <mergeCell ref="D95:E95"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="D104:E104"/>
@@ -2904,8 +2932,8 @@
     <mergeCell ref="D87:E87"/>
     <mergeCell ref="D122:E122"/>
     <mergeCell ref="A126:E126"/>
+    <mergeCell ref="A140:E140"/>
     <mergeCell ref="D121:E121"/>
-    <mergeCell ref="A140:E140"/>
     <mergeCell ref="D74:E74"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="D68:E68"/>

</xml_diff>

<commit_message>
Adicionado Pagina HOME, menu lateral, e pagina responsiva carregando sempre dentro do mesmo layout sem carregar a pagina
</commit_message>
<xml_diff>
--- a/gerados/anexo_f_preenchido.xlsx
+++ b/gerados/anexo_f_preenchido.xlsx
@@ -701,8 +701,8 @@
   </sheetPr>
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:C27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -749,7 +749,7 @@
       </c>
       <c r="B4" s="20" t="inlineStr">
         <is>
-          <t>Joao marques Rantary</t>
+          <t>Fernando da Silva Marques</t>
         </is>
       </c>
       <c r="C4" s="41" t="n"/>
@@ -765,7 +765,7 @@
       </c>
       <c r="B5" s="20" t="inlineStr">
         <is>
-          <t>446.790.168-09</t>
+          <t>172.149.418-99</t>
         </is>
       </c>
       <c r="C5" s="41" t="n"/>
@@ -781,7 +781,7 @@
       </c>
       <c r="B6" s="20" t="inlineStr">
         <is>
-          <t>#UC</t>
+          <t>25837648</t>
         </is>
       </c>
       <c r="C6" s="41" t="n"/>
@@ -797,7 +797,7 @@
       </c>
       <c r="B7" s="20" t="inlineStr">
         <is>
-          <t>Avenida São José do Rio Preto, 3730</t>
+          <t>AVENIDA CINCO A - VIVENDAS BOM JD, 302</t>
         </is>
       </c>
       <c r="C7" s="41" t="n"/>
@@ -813,7 +813,7 @@
       </c>
       <c r="B8" s="20" t="inlineStr">
         <is>
-          <t>#CEP</t>
+          <t>14790-000</t>
         </is>
       </c>
       <c r="C8" s="41" t="n"/>
@@ -829,7 +829,7 @@
       </c>
       <c r="B9" s="20" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>Guaíra</t>
         </is>
       </c>
       <c r="C9" s="41" t="n"/>
@@ -845,7 +845,7 @@
       </c>
       <c r="B10" s="20" t="inlineStr">
         <is>
-          <t>#LAT</t>
+          <t>-20.313673</t>
         </is>
       </c>
       <c r="C10" s="41" t="n"/>
@@ -861,7 +861,7 @@
       </c>
       <c r="B11" s="20" t="inlineStr">
         <is>
-          <t>#LONG</t>
+          <t>-48.308502</t>
         </is>
       </c>
       <c r="C11" s="41" t="n"/>
@@ -877,7 +877,7 @@
       </c>
       <c r="B12" s="20" t="inlineStr">
         <is>
-          <t>#TEL</t>
+          <t>1799978600</t>
         </is>
       </c>
       <c r="C12" s="41" t="n"/>
@@ -893,7 +893,7 @@
       </c>
       <c r="B13" s="20" t="inlineStr">
         <is>
-          <t>#CEL</t>
+          <t>marquefe14@gmail.com</t>
         </is>
       </c>
       <c r="C13" s="41" t="n"/>
@@ -1594,7 +1594,7 @@
       </c>
       <c r="B61" s="38" t="inlineStr">
         <is>
-          <t>ASTRONERGY</t>
+          <t>HELIUS</t>
         </is>
       </c>
       <c r="C61" s="38" t="n"/>
@@ -1610,7 +1610,7 @@
       </c>
       <c r="B62" s="38" t="inlineStr">
         <is>
-          <t>#MODMOD</t>
+          <t>HMF132T12R 600W</t>
         </is>
       </c>
       <c r="C62" s="38" t="n"/>
@@ -1673,7 +1673,7 @@
       </c>
       <c r="B66" s="38" t="inlineStr">
         <is>
-          <t>SUN2000-G3-US-220</t>
+          <t>SUN-M220/225G4-EU-Q0 2.25KW</t>
         </is>
       </c>
       <c r="C66" s="38" t="n"/>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="B67" s="38" t="inlineStr">
         <is>
-          <t>600.0</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="C67" s="38" t="n"/>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="B68" s="38" t="inlineStr">
         <is>
-          <t>2000.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C68" s="38" t="n"/>
@@ -1718,7 +1718,7 @@
       </c>
       <c r="B69" s="38" t="inlineStr">
         <is>
-          <t>05/06/2025</t>
+          <t>03/06/2025</t>
         </is>
       </c>
       <c r="C69" s="38" t="n"/>
@@ -2111,7 +2111,7 @@
       <c r="C102" s="38" t="n"/>
       <c r="D102" s="23" t="inlineStr">
         <is>
-          <t>ASTRONERGY , #MODMOD</t>
+          <t>HELIUS , HMF132T12R 600W</t>
         </is>
       </c>
       <c r="E102" s="40" t="n"/>
@@ -2126,7 +2126,7 @@
       <c r="C103" s="38" t="n"/>
       <c r="D103" s="23" t="inlineStr">
         <is>
-          <t>600.0</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="E103" s="40" t="n"/>
@@ -2154,7 +2154,7 @@
       <c r="C105" s="38" t="n"/>
       <c r="D105" s="23" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="E105" s="40" t="n"/>
@@ -2184,7 +2184,7 @@
       <c r="C107" s="38" t="n"/>
       <c r="D107" s="23" t="inlineStr">
         <is>
-          <t>05/06/2025</t>
+          <t>03/06/2025</t>
         </is>
       </c>
       <c r="E107" s="40" t="n"/>
@@ -2353,7 +2353,7 @@
       <c r="C122" s="38" t="n"/>
       <c r="D122" s="23" t="inlineStr">
         <is>
-          <t>DEYE , SUN2000-G3-US-220</t>
+          <t>DEYE , SUN-M220/225G4-EU-Q0 2.25KW</t>
         </is>
       </c>
       <c r="E122" s="40" t="n"/>
@@ -2383,7 +2383,7 @@
       <c r="C124" s="38" t="n"/>
       <c r="D124" s="23" t="inlineStr">
         <is>
-          <t>2000.0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E124" s="40" t="n"/>

</xml_diff>